<commit_message>
Melhorando o gráfico de dispersão
</commit_message>
<xml_diff>
--- a/ExcelPython4.xlsx
+++ b/ExcelPython4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2022\Python com Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F9896F-B8B6-430B-B855-5B5E7A39D1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32FFBDC-584B-44B5-9C45-70A09B12C89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AD2AD1B6-765F-4264-B12F-D7C6C7F00919}"/>
+    <workbookView xWindow="4980" yWindow="1665" windowWidth="14430" windowHeight="8940" xr2:uid="{AD2AD1B6-765F-4264-B12F-D7C6C7F00919}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,17 +39,17 @@
     <t>Media l(mm)</t>
   </si>
   <si>
-    <t>DesvioPadrao</t>
+    <t>DesvioPadrao F</t>
   </si>
   <si>
-    <t>Desvio Padrão</t>
+    <t>Desvio Padrão l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +64,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -73,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -133,32 +141,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -170,13 +162,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1121,15 +1113,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1457,35 +1449,36 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>3</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>9.1999999999999993</v>
       </c>
       <c r="C2" s="7">
@@ -1504,10 +1497,10 @@
       <c r="B3" s="2">
         <v>12.2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1518,11 +1511,11 @@
       <c r="B4" s="2">
         <v>15</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="8">
         <f>_xlfn.STDEV.S(A2:A8)</f>
         <v>8.5579258724351686</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="8">
         <f>_xlfn.STDEV.S(B2:B8)</f>
         <v>25.530532607803057</v>
       </c>
@@ -1564,23 +1557,15 @@
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>